<commit_message>
updated performance results, fixed wrong names in benchmarks
</commit_message>
<xml_diff>
--- a/Code/Light.GuardClauses.Tests/Performance Test Results.xlsx
+++ b/Code/Light.GuardClauses.Tests/Performance Test Results.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
   <si>
     <t>100ms</t>
   </si>
@@ -50,20 +50,26 @@
     <t>3000ms</t>
   </si>
   <si>
-    <t>Average</t>
+    <t>MustNotBeNull Peformance Test - Imperative vs. Light.GuardClauses</t>
   </si>
   <si>
-    <t>Conducted</t>
+    <t>FluentAssertions</t>
   </si>
   <si>
-    <t>MustNotBeNull Peformance Test - Imperative vs. Light.GuardClauses</t>
+    <t>Average per ms</t>
+  </si>
+  <si>
+    <t>Macrobenchmark</t>
+  </si>
+  <si>
+    <t>Microbenchmark</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -74,6 +80,14 @@
     <font>
       <b/>
       <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -100,12 +114,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -158,8 +173,13 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="de-DE"/>
-              <a:t>Must Not Be Null Performance</a:t>
+              <a:t>MustNot</a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="de-DE" baseline="0"/>
+              <a:t>BeNull Microbenchmark</a:t>
+            </a:r>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -194,16 +214,27 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.19516426071741033"/>
+          <c:y val="9.8150217256362512E-2"/>
+          <c:w val="0.78261351706036741"/>
+          <c:h val="0.78745279745059804"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>MustNotBeNull!$B$2</c:f>
+              <c:f>MustNotBeNull!$B$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -213,11 +244,34 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="34925" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent6">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent6">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst>
               <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
@@ -227,12 +281,10 @@
               </a:outerShdw>
             </a:effectLst>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>MustNotBeNull!$A$3:$A$8</c:f>
+              <c:f>MustNotBeNull!$A$4:$A$9</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -258,35 +310,34 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>MustNotBeNull!$B$3:$B$8</c:f>
+              <c:f>MustNotBeNull!$B$4:$B$9</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>171075022</c:v>
+                  <c:v>55117244</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>706014694</c:v>
+                  <c:v>225776186</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1251158718</c:v>
+                  <c:v>384377196</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1768440306</c:v>
+                  <c:v>548168171</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3564676782</c:v>
+                  <c:v>1098645376</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5346006018</c:v>
+                  <c:v>1633778757</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-5AEB-4C63-89E9-4572974546A3}"/>
+              <c16:uniqueId val="{00000000-6EC0-47D8-936E-F804996D471F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -295,7 +346,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>MustNotBeNull!$C$2</c:f>
+              <c:f>MustNotBeNull!$C$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -305,11 +356,34 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="34925" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent5">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent5">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst>
               <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
@@ -319,12 +393,10 @@
               </a:outerShdw>
             </a:effectLst>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>MustNotBeNull!$A$3:$A$8</c:f>
+              <c:f>MustNotBeNull!$A$4:$A$9</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -350,35 +422,146 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>MustNotBeNull!$C$3:$C$8</c:f>
+              <c:f>MustNotBeNull!$C$4:$C$9</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>44238900</c:v>
+                  <c:v>43330061</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>159170739</c:v>
+                  <c:v>154526266</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>280727837</c:v>
+                  <c:v>279431597</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>390699270</c:v>
+                  <c:v>391201068</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>798348174</c:v>
+                  <c:v>776131828</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1177678419</c:v>
+                  <c:v>1155011900</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-5AEB-4C63-89E9-4572974546A3}"/>
+              <c16:uniqueId val="{00000001-6EC0-47D8-936E-F804996D471F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>MustNotBeNull!$D$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>FluentAssertions</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent4">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent4">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>MustNotBeNull!$A$4:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>100ms</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>400ms</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>700ms</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000ms</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2000ms</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3000ms</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>MustNotBeNull!$D$4:$D$9</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>537055</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2093011</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3575788</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5078955</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10246475</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15384669</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-6EC0-47D8-936E-F804996D471F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -390,12 +573,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="439339920"/>
-        <c:axId val="439340248"/>
-      </c:lineChart>
+        <c:gapWidth val="100"/>
+        <c:overlap val="-24"/>
+        <c:axId val="347886992"/>
+        <c:axId val="347884040"/>
+      </c:barChart>
       <c:catAx>
-        <c:axId val="439339920"/>
+        <c:axId val="347886992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -438,7 +622,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="439340248"/>
+        <c:crossAx val="347884040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -446,7 +630,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="439340248"/>
+        <c:axId val="347884040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -497,7 +681,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="439339920"/>
+        <c:crossAx val="347886992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -611,14 +795,14 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Average</a:t>
+              <a:rPr lang="de-DE"/>
+              <a:t>Average per</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Executions per ms</a:t>
+              <a:rPr lang="de-DE" baseline="0"/>
+              <a:t> ms</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -663,11 +847,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>MustNotBeNull!$A$11</c:f>
+              <c:f>MustNotBeNull!$B$11</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Average</c:v>
+                  <c:v>Imperative</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -676,21 +860,21 @@
             <a:gradFill rotWithShape="1">
               <a:gsLst>
                 <a:gs pos="0">
-                  <a:schemeClr val="accent1">
+                  <a:schemeClr val="accent6">
                     <a:satMod val="103000"/>
                     <a:lumMod val="102000"/>
                     <a:tint val="94000"/>
                   </a:schemeClr>
                 </a:gs>
                 <a:gs pos="50000">
-                  <a:schemeClr val="accent1">
+                  <a:schemeClr val="accent6">
                     <a:satMod val="110000"/>
                     <a:lumMod val="100000"/>
                     <a:shade val="100000"/>
                   </a:schemeClr>
                 </a:gs>
                 <a:gs pos="100000">
-                  <a:schemeClr val="accent1">
+                  <a:schemeClr val="accent6">
                     <a:lumMod val="99000"/>
                     <a:satMod val="120000"/>
                     <a:shade val="78000"/>
@@ -711,44 +895,377 @@
             </a:effectLst>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="de-DE"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>MustNotBeNull!$B$10:$C$10</c:f>
+              <c:f>MustNotBeNull!$A$12</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Imperative</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Light.GuardClauses</c:v>
+                  <c:v>Average per ms</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>MustNotBeNull!$B$11:$C$11</c:f>
+              <c:f>MustNotBeNull!$B$12</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1763271.37</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>392284.72</c:v>
+                  <c:v>548244.91</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-5EC5-485B-A693-0681E2FA6884}"/>
+              <c16:uniqueId val="{00000000-0D06-4EB4-BAC9-E499D092658B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>MustNotBeNull!$C$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Light.GuardClauses</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent5">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent5">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="de-DE"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>MustNotBeNull!$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Average per ms</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>MustNotBeNull!$C$12</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>387727.77</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-0D06-4EB4-BAC9-E499D092658B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>MustNotBeNull!$D$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>FluentAssertions</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent4">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent4">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="de-DE"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>MustNotBeNull!$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Average per ms</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>MustNotBeNull!$D$12</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>5094.84</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-0D06-4EB4-BAC9-E499D092658B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -756,11 +1273,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="-24"/>
-        <c:axId val="436922776"/>
-        <c:axId val="436193920"/>
+        <c:axId val="345953240"/>
+        <c:axId val="245877712"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="436922776"/>
+        <c:axId val="345953240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -803,7 +1320,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="436193920"/>
+        <c:crossAx val="245877712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -811,7 +1328,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="436193920"/>
+        <c:axId val="245877712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -862,7 +1379,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="436922776"/>
+        <c:crossAx val="345953240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -874,6 +1391,823 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-DE"/>
+              <a:t>Sorting List&lt;int&gt; with initial reverse order</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>MustNotBeNull!$B$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Imperative</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent6">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent6">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="de-DE"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>MustNotBeNull!$A$16:$A$21</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>400000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>800000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1600000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3200000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>MustNotBeNull!$B$16:$B$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>162</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-988B-4FF8-82DC-5C811ACABB9E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>MustNotBeNull!$C$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Light.GuardClauses</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent5">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent5">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="de-DE"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>MustNotBeNull!$A$16:$A$21</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>400000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>800000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1600000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3200000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>MustNotBeNull!$C$16:$C$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>163</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-988B-4FF8-82DC-5C811ACABB9E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>MustNotBeNull!$D$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>FluentAssertions</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent4">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent4">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="de-DE"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>MustNotBeNull!$A$16:$A$21</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>400000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>800000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1600000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3200000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>MustNotBeNull!$D$16:$D$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>166</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-988B-4FF8-82DC-5C811ACABB9E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="100"/>
+        <c:overlap val="-24"/>
+        <c:axId val="405478168"/>
+        <c:axId val="405478824"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="405478168"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="405478824"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="405478824"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="405478168"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -912,13 +2246,10 @@
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
+  <a:schemeClr val="accent6"/>
+  <a:schemeClr val="accent5"/>
   <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
   <cs:variation/>
   <cs:variation>
     <a:lumMod val="60000"/>
@@ -952,13 +2283,47 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
+  <a:schemeClr val="accent6"/>
+  <a:schemeClr val="accent5"/>
   <a:schemeClr val="accent4"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
+  <a:schemeClr val="accent6"/>
   <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
+  <a:schemeClr val="accent4"/>
   <cs:variation/>
   <cs:variation>
     <a:lumMod val="60000"/>
@@ -992,7 +2357,7 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="342">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="340">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -1098,7 +2463,7 @@
     </cs:fillRef>
     <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
   </cs:dataPoint>
   <cs:dataPoint3D>
@@ -1108,7 +2473,7 @@
     </cs:fillRef>
     <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
   </cs:dataPoint3D>
   <cs:dataPointLine>
@@ -1118,7 +2483,7 @@
     <cs:fillRef idx="3"/>
     <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="34925" cap="rnd">
@@ -1138,7 +2503,7 @@
     </cs:fillRef>
     <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
@@ -1157,7 +2522,7 @@
     <cs:fillRef idx="3"/>
     <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -1995,24 +3360,526 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="340">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>14287</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>319087</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2029,20 +3896,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>52387</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>4762</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>266699</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>357187</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>309562</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvPr id="6" name="Chart 5"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2052,6 +3919,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>604837</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>180974</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2357,123 +4254,249 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16" customWidth="1"/>
     <col min="2" max="2" width="14.5703125" customWidth="1"/>
     <col min="3" max="3" width="18.28515625" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="1">
+        <v>55117244</v>
+      </c>
+      <c r="C4" s="1">
+        <v>43330061</v>
+      </c>
+      <c r="D4" s="1">
+        <v>537055</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1">
+        <v>225776186</v>
+      </c>
+      <c r="C5" s="1">
+        <v>154526266</v>
+      </c>
+      <c r="D5" s="1">
+        <v>2093011</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1">
+        <v>384377196</v>
+      </c>
+      <c r="C6" s="1">
+        <v>279431597</v>
+      </c>
+      <c r="D6" s="1">
+        <v>3575788</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="1">
+        <v>548168171</v>
+      </c>
+      <c r="C7" s="1">
+        <v>391201068</v>
+      </c>
+      <c r="D7" s="1">
+        <v>5078955</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1098645376</v>
+      </c>
+      <c r="C8" s="1">
+        <v>776131828</v>
+      </c>
+      <c r="D8" s="1">
+        <v>10246475</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1633778757</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1155011900</v>
+      </c>
+      <c r="D9" s="1">
+        <v>15384669</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>10</v>
       </c>
+      <c r="B12" s="2">
+        <v>548244.91</v>
+      </c>
+      <c r="C12" s="2">
+        <v>387727.77</v>
+      </c>
+      <c r="D12" s="2">
+        <v>5094.84</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+    <row r="14" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="3"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C15" t="s">
         <v>5</v>
       </c>
+      <c r="D15" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="1">
-        <v>171075022</v>
-      </c>
-      <c r="C3" s="1">
-        <v>44238900</v>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>100000</v>
+      </c>
+      <c r="B16">
+        <v>6</v>
+      </c>
+      <c r="C16">
+        <v>4</v>
+      </c>
+      <c r="D16">
+        <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="1">
-        <v>706014694</v>
-      </c>
-      <c r="C4" s="1">
-        <v>159170739</v>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>200000</v>
+      </c>
+      <c r="B17">
+        <v>8</v>
+      </c>
+      <c r="C17">
+        <v>8</v>
+      </c>
+      <c r="D17">
+        <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="1">
-        <v>1251158718</v>
-      </c>
-      <c r="C5" s="1">
-        <v>280727837</v>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>400000</v>
+      </c>
+      <c r="B18">
+        <v>17</v>
+      </c>
+      <c r="C18">
+        <v>17</v>
+      </c>
+      <c r="D18">
+        <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="1">
-        <v>1768440306</v>
-      </c>
-      <c r="C6" s="1">
-        <v>390699270</v>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>800000</v>
+      </c>
+      <c r="B19">
+        <v>37</v>
+      </c>
+      <c r="C19">
+        <v>37</v>
+      </c>
+      <c r="D19">
+        <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1">
-        <v>3564676782</v>
-      </c>
-      <c r="C7" s="1">
-        <v>798348174</v>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>1600000</v>
+      </c>
+      <c r="B20">
+        <v>78</v>
+      </c>
+      <c r="C20">
+        <v>76</v>
+      </c>
+      <c r="D20">
+        <v>77</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1">
-        <v>5346006018</v>
-      </c>
-      <c r="C8" s="1">
-        <v>1177678419</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="2">
-        <v>1763271.37</v>
-      </c>
-      <c r="C11" s="2">
-        <v>392284.72</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="3">
-        <v>42516</v>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>3200000</v>
+      </c>
+      <c r="B21">
+        <v>162</v>
+      </c>
+      <c r="C21">
+        <v>163</v>
+      </c>
+      <c r="D21">
+        <v>166</v>
       </c>
     </row>
   </sheetData>

</xml_diff>